<commit_message>
made changes to template files to include ID to blog page added in pytest selenium test cases modified some test scenario names in the test cases.xlsx
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\Week 4\ETI CA1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77653F96-24E7-4B4B-8A17-0A50459735F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF4B99B-2158-4D3A-AF4B-64D6CC46AACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{5FFF84C8-027C-44D2-9C9A-FE84A56D8A59}"/>
+    <workbookView xWindow="19065" yWindow="4050" windowWidth="21600" windowHeight="11055" xr2:uid="{5FFF84C8-027C-44D2-9C9A-FE84A56D8A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,18 +51,9 @@
     <t>Viewing Home page</t>
   </si>
   <si>
-    <t>Viewing list of posts with a particular category</t>
-  </si>
-  <si>
     <t>Leaving a comment</t>
   </si>
   <si>
-    <t>Leaving a comment without entering the name</t>
-  </si>
-  <si>
-    <t>Leaving a comment without entering the comment body</t>
-  </si>
-  <si>
     <t>This is to test if the Home page can be viewed successfully.</t>
   </si>
   <si>
@@ -76,9 +67,6 @@
   </si>
   <si>
     <t>This is to test if there will be an error message when a comment without a body is submitted.</t>
-  </si>
-  <si>
-    <t>Leaving a comment with a name of more than 60 characters</t>
   </si>
   <si>
     <t>This is to test if the author of the comment can be more than 60 characters.</t>
@@ -199,6 +187,18 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Viewing list of posts by category</t>
+  </si>
+  <si>
+    <t>Leaving a comment with the author more than 60 characters</t>
+  </si>
+  <si>
+    <t>Leaving a comment without an author</t>
+  </si>
+  <si>
+    <t>Leaving a comment without a body</t>
   </si>
 </sst>
 </file>
@@ -590,21 +590,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8836015B-E344-4C03-9F7A-1A503866889C}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.703125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="33.5859375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="36.29296875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.5859375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.41015625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.1171875" style="2"/>
+    <col min="1" max="1" width="22.7109375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="33.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -621,165 +621,165 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="123" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="10" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "made changes to template files to include ID to blog page"
This reverts commit 0a304ed20a5f255a9d1365649c3b37b0f7831aac.
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\Week 4\ETI CA1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF4B99B-2158-4D3A-AF4B-64D6CC46AACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77653F96-24E7-4B4B-8A17-0A50459735F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19065" yWindow="4050" windowWidth="21600" windowHeight="11055" xr2:uid="{5FFF84C8-027C-44D2-9C9A-FE84A56D8A59}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{5FFF84C8-027C-44D2-9C9A-FE84A56D8A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,18 @@
     <t>Viewing Home page</t>
   </si>
   <si>
+    <t>Viewing list of posts with a particular category</t>
+  </si>
+  <si>
     <t>Leaving a comment</t>
   </si>
   <si>
+    <t>Leaving a comment without entering the name</t>
+  </si>
+  <si>
+    <t>Leaving a comment without entering the comment body</t>
+  </si>
+  <si>
     <t>This is to test if the Home page can be viewed successfully.</t>
   </si>
   <si>
@@ -67,6 +76,9 @@
   </si>
   <si>
     <t>This is to test if there will be an error message when a comment without a body is submitted.</t>
+  </si>
+  <si>
+    <t>Leaving a comment with a name of more than 60 characters</t>
   </si>
   <si>
     <t>This is to test if the author of the comment can be more than 60 characters.</t>
@@ -187,18 +199,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Viewing list of posts by category</t>
-  </si>
-  <si>
-    <t>Leaving a comment with the author more than 60 characters</t>
-  </si>
-  <si>
-    <t>Leaving a comment without an author</t>
-  </si>
-  <si>
-    <t>Leaving a comment without a body</t>
   </si>
 </sst>
 </file>
@@ -590,21 +590,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8836015B-E344-4C03-9F7A-1A503866889C}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="33.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="22.703125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="33.5859375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.29296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.5859375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.41015625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.1171875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -621,165 +621,165 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="123" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="71.7" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added in new test cases 1. scrolling in website 2. redirection in website
</commit_message>
<xml_diff>
--- a/test cases.xlsx
+++ b/test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\Week 4\ETI CA1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF4B99B-2158-4D3A-AF4B-64D6CC46AACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E8DCC0-82A6-4201-AC67-3711F8D1C575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19065" yWindow="4050" windowWidth="21600" windowHeight="11055" xr2:uid="{5FFF84C8-027C-44D2-9C9A-FE84A56D8A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5FFF84C8-027C-44D2-9C9A-FE84A56D8A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>The value shown in the author name text field should only be "ABCDEFGHIJKLMNOPQRSTUVWXYZABCDEFGHIJKLMNOPQRSTUVWXYZABCDEFGH" and is missing an "I".</t>
-  </si>
-  <si>
-    <t>At the body text field, there will be an error prompt which says "Please fill out this field."</t>
-  </si>
-  <si>
-    <t>At the author name text field, there will be an error prompt which says "Please fill out this field."</t>
   </si>
   <si>
     <t>Test Steps</t>
@@ -199,6 +193,40 @@
   </si>
   <si>
     <t>Leaving a comment without a body</t>
+  </si>
+  <si>
+    <t>Same as expected outcome.</t>
+  </si>
+  <si>
+    <t>At the author name field, there will be an error when trying to submit the form since the field is invalid.</t>
+  </si>
+  <si>
+    <t>At the body text field, there will be an error when trying to submit the form since the field is invalid.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>This is to test if scrolling can be done successfully.</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost:8000/projects
+2. Scroll to the bottom of the page.</t>
+  </si>
+  <si>
+    <t>The page should scroll down to the bottom.</t>
+  </si>
+  <si>
+    <t>Redirection in the website</t>
+  </si>
+  <si>
+    <t>This is to test if redirection in the website can be done successfully.</t>
+  </si>
+  <si>
+    <t>Scrolling in the website</t>
+  </si>
+  <si>
+    <t>The page should load successfully and display the "Blog" page.</t>
   </si>
 </sst>
 </file>
@@ -588,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8836015B-E344-4C03-9F7A-1A503866889C}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -638,148 +666,226 @@
         <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="F5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="F10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>